<commit_message>
- Make CN-Wheat chart to work - add some graphs and postprocessing in scenarii_monoculms
</commit_message>
<xml_diff>
--- a/branches/multirun/example/Scenarii_monoculms/inputs/Generate_inputs.xlsx
+++ b/branches/multirun/example/Scenarii_monoculms/inputs/Generate_inputs.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
     <sheet name="Fit leaf_L" sheetId="21" r:id="rId2"/>
+    <sheet name="SL_ratio" sheetId="22" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="162">
   <si>
     <t>plant</t>
   </si>
@@ -651,6 +652,318 @@
   <si>
     <t>internode_Lmax_lig</t>
   </si>
+  <si>
+    <r>
+      <t>parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">SL_ratio_a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">leaf_rank </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">** </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF2D4293"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">SL_ratio_b </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">leaf_rank </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">** </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF2D4293"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">SL_ratio_c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">leaf_rank </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>SL_ratio_d</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">def </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>calculate_SL_ratio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>leaf_rank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0EB242"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>""" Sheath:Lamina final length ratio according to the rank. Parameters from Dornbush (2011).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SL_ratio_a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL_ratio_b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL_ratio_c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL_ratio_d </t>
+  </si>
+  <si>
+    <t>SLratio_Vmodel</t>
+  </si>
+  <si>
+    <t>SLratio_Vnew</t>
+  </si>
+  <si>
+    <t>SLratio_Vnew2</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +975,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,6 +1124,51 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000066"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF2D4293"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFA0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000066"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0EB242"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1077,7 +1435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1211,6 +1569,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1220,7 +1591,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,7 +1624,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1595,7 +1964,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1941,6 +2309,648 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>SL ratio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SL_ratio!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SLratio_Vmodel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SL_ratio!$A$13:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SL_ratio!$B$13:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.37839999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31439999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39519999999999977</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45839999999999981</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5673999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.58799999999999986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56919999999999948</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.49839999999999973</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36299999999999977</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15040000000000031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.15199999999999969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EE06-481C-BAC0-5898482901C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SL_ratio!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SLratio_Vnew</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SL_ratio!$A$13:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SL_ratio!$C$13:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.26762999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28526000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30288999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32052000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33815000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35577999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37341000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40866999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44392999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46155999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47919</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.49681999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EE06-481C-BAC0-5898482901C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SL_ratio!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SLratio_Vnew2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SL_ratio!$A$13:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SL_ratio!$D$13:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.432</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.44400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.45599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.46799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EE06-481C-BAC0-5898482901C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1219627551"/>
+        <c:axId val="1219613823"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1219627551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>SL_ratio!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>metamer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1219613823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1219613823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>SL ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1219627551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -3138,6 +4148,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -3406,7 +4451,7 @@
   </sheetPr>
   <dimension ref="A1:BH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -3463,7 +4508,7 @@
       </c>
     </row>
     <row r="4" spans="1:60" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="96" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3643,7 +4688,7 @@
       </c>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A5" s="91"/>
+      <c r="A5" s="96"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -3737,19 +4782,19 @@
         <v>33</v>
       </c>
       <c r="AE5" s="1">
-        <f>AK5*$AV$15</f>
+        <f t="shared" ref="AE5:AE12" si="0">AK5*$AV$15</f>
         <v>8.9088436646547198</v>
       </c>
       <c r="AF5" s="1">
-        <f>AK5*$AX5</f>
+        <f t="shared" ref="AF5:AF12" si="1">AK5*$AX5</f>
         <v>0.99652622317307915</v>
       </c>
       <c r="AG5" s="24">
-        <f>AK5*$BA5</f>
+        <f t="shared" ref="AG5:AG12" si="2">AK5*$BA5</f>
         <v>8.9088436646547198</v>
       </c>
       <c r="AH5" s="26">
-        <f>AK5*$AY5</f>
+        <f t="shared" ref="AH5:AH12" si="3">AK5*$AY5</f>
         <v>9.9652622317307902</v>
       </c>
       <c r="AI5" s="1">
@@ -3796,29 +4841,29 @@
         <v>32</v>
       </c>
       <c r="AU5" s="55">
-        <f>AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
+        <f t="shared" ref="AU5:AU12" si="4">AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
         <v>3.3011513455652687E-3</v>
       </c>
       <c r="AV5" s="56">
-        <f>(1-AK5/AU5)*100</f>
+        <f t="shared" ref="AV5:AV12" si="5">(1-AK5/AU5)*100</f>
         <v>38.829284515098252</v>
       </c>
       <c r="AW5" s="13">
         <v>4.5999999999999996</v>
       </c>
       <c r="AX5" s="13">
-        <f>(($AW5/100)*(1+($AV$15+$BA5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW5/100))</f>
+        <f t="shared" ref="AX5:AX12" si="6">(($AW5/100)*(1+($AV$15+$BA5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW5/100))</f>
         <v>493.49156696102204</v>
       </c>
       <c r="AY5" s="13">
-        <f>$AX5/$X$23</f>
+        <f t="shared" ref="AY5:AY12" si="7">$AX5/$X$23</f>
         <v>4934.91566961022</v>
       </c>
       <c r="AZ5" s="13">
         <v>10</v>
       </c>
       <c r="BA5" s="68">
-        <f>$AZ5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" ref="BA5:BA12" si="8">$AZ5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
       <c r="BB5" s="7">
@@ -3829,7 +4874,7 @@
         <v>9.1058115591388438E-4</v>
       </c>
       <c r="BD5" s="7">
-        <f>J5*Z5</f>
+        <f t="shared" ref="BD5:BD12" si="9">J5*Z5</f>
         <v>2.6054999999999997E-3</v>
       </c>
       <c r="BE5" s="8">
@@ -3837,17 +4882,17 @@
         <v>2.0180134110471437E-3</v>
       </c>
       <c r="BF5" s="8">
-        <f>$T$27+$T$28*$T$30*(L5)^$T$29</f>
+        <f t="shared" ref="BF5:BF12" si="10">$T$27+$T$28*$T$30*(L5)^$T$29</f>
         <v>4.0277279389003447E-3</v>
       </c>
       <c r="BG5" s="7"/>
       <c r="BH5" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M5)^$BB$21</f>
+        <f t="shared" ref="BH5:BH12" si="11">$BC$20*$BB$22*$BB$24*(M5)^$BB$21</f>
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
+      <c r="A6" s="96"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -3858,7 +4903,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E11" si="0">(10-D6)*$E$2</f>
+        <f t="shared" ref="E6:E11" si="12">(10-D6)*$E$2</f>
         <v>3287520</v>
       </c>
       <c r="F6">
@@ -3878,7 +4923,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="K6" s="36">
-        <f t="shared" ref="K6:K12" si="1">J6-M6</f>
+        <f t="shared" ref="K6:K12" si="13">J6-M6</f>
         <v>2.8930000000000001E-2</v>
       </c>
       <c r="L6" s="36">
@@ -3915,7 +4960,7 @@
         <v>3.3993521965748258E-2</v>
       </c>
       <c r="W6" s="1">
-        <f t="shared" ref="W6:W12" si="2">$W$2*EXP($X$2*E6)</f>
+        <f t="shared" ref="W6:W12" si="14">$W$2*EXP($X$2*E6)</f>
         <v>2.6776375833009532E-5</v>
       </c>
       <c r="X6" t="s">
@@ -3940,19 +4985,19 @@
         <v>33</v>
       </c>
       <c r="AE6" s="1">
-        <f>AK6*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>3.5881220853167113</v>
       </c>
       <c r="AF6" s="1">
-        <f>AK6*$AX6</f>
+        <f t="shared" si="1"/>
         <v>0.67583627559825854</v>
       </c>
       <c r="AG6" s="24">
-        <f>AK6*$BA6</f>
+        <f t="shared" si="2"/>
         <v>1.7940610426583556</v>
       </c>
       <c r="AH6" s="26">
-        <f>AK6*$AY6</f>
+        <f t="shared" si="3"/>
         <v>6.7583627559825858</v>
       </c>
       <c r="AI6" s="1">
@@ -3964,19 +5009,19 @@
         <v>1.6879744031468265E-7</v>
       </c>
       <c r="AK6">
-        <f t="shared" ref="AK6:AK12" si="3">AI6+AJ6</f>
+        <f t="shared" ref="AK6:AK12" si="15">AI6+AJ6</f>
         <v>8.1330767267178783E-4</v>
       </c>
       <c r="AL6">
-        <f t="shared" ref="AL6:AM12" si="4">AI6*0.005</f>
+        <f t="shared" ref="AL6:AM12" si="16">AI6*0.005</f>
         <v>4.0656943761573658E-6</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>8.4398720157341326E-10</v>
       </c>
       <c r="AN6">
-        <f t="shared" ref="AN6:AN12" si="5">AL6+AM6</f>
+        <f t="shared" ref="AN6:AN12" si="17">AL6+AM6</f>
         <v>4.066538363358939E-6</v>
       </c>
       <c r="AO6" s="1">
@@ -3992,36 +5037,36 @@
         <v>33</v>
       </c>
       <c r="AS6" s="1">
-        <f t="shared" ref="AS6:AS12" si="6">T6</f>
+        <f t="shared" ref="AS6:AS12" si="18">T6</f>
         <v>0.1331</v>
       </c>
       <c r="AT6" t="s">
         <v>32</v>
       </c>
       <c r="AU6" s="55">
-        <f>AK6+AE6*$E$31+AF6*$F$31+AH6*$J$31</f>
+        <f t="shared" si="4"/>
         <v>1.612515340843685E-3</v>
       </c>
       <c r="AV6" s="56">
-        <f>(1-AK6/AU6)*100</f>
+        <f t="shared" si="5"/>
         <v>49.562794717583479</v>
       </c>
       <c r="AW6" s="13">
         <v>6.5</v>
       </c>
       <c r="AX6" s="13">
-        <f>(($AW6/100)*(1+($AV$15+$BA6)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW6/100))</f>
+        <f t="shared" si="6"/>
         <v>830.97245766546928</v>
       </c>
       <c r="AY6" s="13">
-        <f>$AX6/$X$23</f>
+        <f t="shared" si="7"/>
         <v>8309.724576654693</v>
       </c>
       <c r="AZ6" s="13">
         <v>5</v>
       </c>
       <c r="BA6" s="68">
-        <f>$AZ6/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>2205.8823529411766</v>
       </c>
       <c r="BB6" s="7">
@@ -4032,7 +5077,7 @@
         <v>9.1017858127080242E-4</v>
       </c>
       <c r="BD6" s="7" t="e">
-        <f>J6*Z6</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE6" s="8" t="e">
@@ -4040,17 +5085,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="BF6" s="8">
-        <f>$T$27+$T$28*$T$30*(L6)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>8.1313887523147316E-4</v>
       </c>
       <c r="BG6" s="7"/>
       <c r="BH6" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M6)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
+      <c r="A7" s="96"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -4061,7 +5106,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2739600</v>
       </c>
       <c r="F7">
@@ -4081,10 +5126,10 @@
         <v>2.894E-2</v>
       </c>
       <c r="K7" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L7" s="94">
+      <c r="L7" s="91">
         <v>1.9677388526365687E-3</v>
       </c>
       <c r="M7" s="36">
@@ -4118,7 +5163,7 @@
         <v>32</v>
       </c>
       <c r="W7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.5480791541095022E-5</v>
       </c>
       <c r="X7" t="s">
@@ -4143,19 +5188,19 @@
         <v>33</v>
       </c>
       <c r="AE7" s="1">
-        <f>AK7*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>0.12873040793583418</v>
       </c>
       <c r="AF7" s="1">
-        <f>AK7*$AX7</f>
+        <f t="shared" si="1"/>
         <v>5.3069049208309536E-2</v>
       </c>
       <c r="AG7" s="24">
-        <f>AK7*$BA7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH7" s="26">
-        <f>AK7*$AY7</f>
+        <f t="shared" si="3"/>
         <v>0.53069049208309527</v>
       </c>
       <c r="AI7" s="1">
@@ -4166,19 +5211,19 @@
         <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.9178892465455746E-5</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>1.4589446232727874E-7</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>1.4589446232727874E-7</v>
       </c>
       <c r="AO7" s="1">
@@ -4194,63 +5239,63 @@
         <v>33</v>
       </c>
       <c r="AS7" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT7" t="s">
         <v>32</v>
       </c>
       <c r="AU7" s="55">
-        <f>AK7+AE7*$E$31+AF7*$F$31+AH7*$J$31</f>
+        <f t="shared" si="4"/>
         <v>8.7563453056915228E-5</v>
       </c>
       <c r="AV7" s="56">
-        <f>(1-AK7/AU7)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW7" s="13">
         <v>9.5</v>
       </c>
       <c r="AX7" s="13">
-        <f>(($AW7/100)*(1+($AV$15+$BA7)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW7/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY7" s="13">
-        <f>$AX7/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ7" s="13">
         <v>0</v>
       </c>
       <c r="BA7" s="68">
-        <f>$AZ7/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB7" s="7"/>
       <c r="BC7" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
+        <f t="shared" ref="BC7:BC12" si="19">$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
         <v>#VALUE!</v>
       </c>
       <c r="BD7" s="7" t="e">
-        <f>J7*Z7</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE7" s="8" t="e">
-        <f>BC7+((BD7-BC7)/$T$31)*F7</f>
+        <f t="shared" ref="BE7:BE12" si="20">BC7+((BD7-BC7)/$T$31)*F7</f>
         <v>#VALUE!</v>
       </c>
       <c r="BF7" s="8">
-        <f>$T$27+$T$28*$T$30*(L7)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.9178892465455746E-5</v>
       </c>
       <c r="BG7" s="7"/>
       <c r="BH7" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M7)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
+      <c r="A8" s="96"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -4261,7 +5306,7 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2191680</v>
       </c>
       <c r="F8">
@@ -4277,14 +5322,14 @@
         <v>33</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J12" si="7">J7-M8</f>
+        <f t="shared" ref="J8:J12" si="21">J7-M8</f>
         <v>2.894E-2</v>
       </c>
       <c r="K8" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L8" s="94">
+      <c r="L8" s="91">
         <v>7.5411160325070082E-4</v>
       </c>
       <c r="M8" s="36">
@@ -4318,7 +5363,7 @@
         <v>32</v>
       </c>
       <c r="W8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>8.9502368891684043E-6</v>
       </c>
       <c r="X8" t="s">
@@ -4343,42 +5388,42 @@
         <v>33</v>
       </c>
       <c r="AE8" s="1">
-        <f>AK8*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>3.7798204342272199E-2</v>
       </c>
       <c r="AF8" s="1">
-        <f>AK8*$AX8</f>
+        <f t="shared" si="1"/>
         <v>1.5582291693083372E-2</v>
       </c>
       <c r="AG8" s="24">
-        <f>AK8*$BA8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH8" s="26">
-        <f>AK8*$AY8</f>
+        <f t="shared" si="3"/>
         <v>0.15582291693083369</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" ref="AI8:AI12" si="8">BF8</f>
+        <f t="shared" ref="AI8:AI12" si="22">BF8</f>
         <v>8.5675929842483652E-6</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>8.5675929842483652E-6</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>4.2837964921241826E-8</v>
       </c>
       <c r="AM8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>4.2837964921241826E-8</v>
       </c>
       <c r="AO8" t="s">
@@ -4394,63 +5439,63 @@
         <v>33</v>
       </c>
       <c r="AS8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT8" t="s">
         <v>32</v>
       </c>
       <c r="AU8" s="55">
-        <f>AK8+AE8*$E$31+AF8*$F$31+AH8*$J$31</f>
+        <f t="shared" si="4"/>
         <v>2.5710640901642957E-5</v>
       </c>
       <c r="AV8" s="56">
-        <f>(1-AK8/AU8)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW8" s="13">
         <v>9.5</v>
       </c>
       <c r="AX8" s="13">
-        <f>(($AW8/100)*(1+($AV$15+$BA8)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW8/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY8" s="13">
-        <f>$AX8/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ8" s="13">
         <v>0</v>
       </c>
       <c r="BA8" s="68">
-        <f>$AZ8/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB8" s="7"/>
       <c r="BC8" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T8*$T$32)^$T$29</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BD8" s="7" t="e">
-        <f>J8*Z8</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE8" s="8" t="e">
-        <f>BC8+((BD8-BC8)/$T$31)*F8</f>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="BF8" s="8">
-        <f>$T$27+$T$28*$T$30*(L8)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>8.5675929842483652E-6</v>
       </c>
       <c r="BG8" s="7"/>
       <c r="BH8" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M8)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A9" s="91"/>
+      <c r="A9" s="96"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -4461,7 +5506,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1643760</v>
       </c>
       <c r="F9">
@@ -4477,14 +5522,14 @@
         <v>33</v>
       </c>
       <c r="J9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.894E-2</v>
       </c>
       <c r="K9" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L9" s="94">
+      <c r="L9" s="91">
         <v>3.1376376813217782E-4</v>
       </c>
       <c r="M9" s="36">
@@ -4518,7 +5563,7 @@
         <v>32</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>5.1745894361784425E-6</v>
       </c>
       <c r="X9" t="s">
@@ -4543,42 +5588,42 @@
         <v>33</v>
       </c>
       <c r="AE9" s="1">
-        <f>AK9*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>1.2381691922498196E-2</v>
       </c>
       <c r="AF9" s="1">
-        <f>AK9*$AX9</f>
+        <f t="shared" si="1"/>
         <v>5.1043465833240436E-3</v>
       </c>
       <c r="AG9" s="24">
-        <f>AK9*$BA9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH9" s="26">
-        <f>AK9*$AY9</f>
+        <f t="shared" si="3"/>
         <v>5.1043465833240424E-2</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>2.8065168357662577E-6</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.8065168357662577E-6</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>1.4032584178831289E-8</v>
       </c>
       <c r="AM9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>1.4032584178831289E-8</v>
       </c>
       <c r="AO9" t="s">
@@ -4594,63 +5639,63 @@
         <v>33</v>
       </c>
       <c r="AS9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT9" t="s">
         <v>32</v>
       </c>
       <c r="AU9" s="55">
-        <f>AK9+AE9*$E$31+AF9*$F$31+AH9*$J$31</f>
+        <f t="shared" si="4"/>
         <v>8.4221258737971998E-6</v>
       </c>
       <c r="AV9" s="56">
-        <f>(1-AK9/AU9)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW9" s="13">
         <v>9.5</v>
       </c>
       <c r="AX9" s="13">
-        <f>(($AW9/100)*(1+($AV$15+$BA9)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW9/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY9" s="13">
-        <f>$AX9/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ9" s="13">
         <v>0</v>
       </c>
       <c r="BA9" s="68">
-        <f>$AZ9/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB9" s="7"/>
       <c r="BC9" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T9*$T$32)^$T$29</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BD9" s="7" t="e">
-        <f>J9*Z9</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE9" s="8" t="e">
-        <f>BC9+((BD9-BC9)/$T$31)*F9</f>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="BF9" s="8">
-        <f>$T$27+$T$28*$T$30*(L9)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.8065168357662577E-6</v>
       </c>
       <c r="BG9" s="7"/>
       <c r="BH9" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M9)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
+      <c r="A10" s="96"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -4661,7 +5706,7 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1095840</v>
       </c>
       <c r="F10">
@@ -4677,14 +5722,14 @@
         <v>33</v>
       </c>
       <c r="J10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.894E-2</v>
       </c>
       <c r="K10" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L10" s="94">
+      <c r="L10" s="91">
         <v>1.4587358230165945E-4</v>
       </c>
       <c r="M10" s="36">
@@ -4718,7 +5763,7 @@
         <v>32</v>
       </c>
       <c r="W10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>2.9916946517264094E-6</v>
       </c>
       <c r="X10" t="s">
@@ -4743,42 +5788,42 @@
         <v>33</v>
       </c>
       <c r="AE10" s="1">
-        <f>AK10*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>4.7183998739784598E-3</v>
       </c>
       <c r="AF10" s="1">
-        <f>AK10*$AX10</f>
+        <f t="shared" si="1"/>
         <v>1.9451580952144349E-3</v>
       </c>
       <c r="AG10" s="24">
-        <f>AK10*$BA10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH10" s="26">
-        <f>AK10*$AY10</f>
+        <f t="shared" si="3"/>
         <v>1.9451580952144346E-2</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>1.0695039714351174E-6</v>
       </c>
       <c r="AJ10" s="1">
         <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>1.0695039714351174E-6</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>5.3475198571755876E-9</v>
       </c>
       <c r="AM10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>5.3475198571755876E-9</v>
       </c>
       <c r="AO10" t="s">
@@ -4794,63 +5839,63 @@
         <v>33</v>
       </c>
       <c r="AS10" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT10" t="s">
         <v>32</v>
       </c>
       <c r="AU10" s="55">
-        <f>AK10+AE10*$E$31+AF10*$F$31+AH10*$J$31</f>
+        <f t="shared" si="4"/>
         <v>3.2094933317915637E-6</v>
       </c>
       <c r="AV10" s="56">
-        <f>(1-AK10/AU10)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW10" s="13">
         <v>9.5</v>
       </c>
       <c r="AX10" s="13">
-        <f>(($AW10/100)*(1+($AV$15+$BA10)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW10/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY10" s="13">
-        <f>$AX10/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ10" s="13">
         <v>0</v>
       </c>
       <c r="BA10" s="68">
-        <f>$AZ10/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB10" s="7"/>
       <c r="BC10" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T10*$T$32)^$T$29</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BD10" s="7" t="e">
-        <f>J10*Z10</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE10" s="8" t="e">
-        <f>BC10+((BD10-BC10)/$T$31)*F10</f>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="BF10" s="8">
-        <f>$T$27+$T$28*$T$30*(L10)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>1.0695039714351174E-6</v>
       </c>
       <c r="BG10" s="7"/>
       <c r="BH10" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M10)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
+      <c r="A11" s="96"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -4861,7 +5906,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>547920</v>
       </c>
       <c r="F11">
@@ -4877,14 +5922,14 @@
         <v>33</v>
       </c>
       <c r="J11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.894E-2</v>
       </c>
       <c r="K11" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L11" s="94">
+      <c r="L11" s="91">
         <v>7.7994660715105795E-5</v>
       </c>
       <c r="M11" s="36">
@@ -4918,7 +5963,7 @@
         <v>32</v>
       </c>
       <c r="W11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.7296515983649451E-6</v>
       </c>
       <c r="X11" t="s">
@@ -4943,42 +5988,42 @@
         <v>33</v>
       </c>
       <c r="AE11" s="1">
-        <f>AK11*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>2.1815845434399943E-3</v>
       </c>
       <c r="AF11" s="1">
-        <f>AK11*$AX11</f>
+        <f t="shared" si="1"/>
         <v>8.9935718642026317E-4</v>
       </c>
       <c r="AG11" s="24">
-        <f>AK11*$BA11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH11" s="26">
-        <f>AK11*$AY11</f>
+        <f t="shared" si="3"/>
         <v>8.9935718642026301E-3</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>4.944924965130653E-7</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>4.944924965130653E-7</v>
       </c>
       <c r="AL11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>2.4724624825653264E-9</v>
       </c>
       <c r="AM11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>2.4724624825653264E-9</v>
       </c>
       <c r="AO11" t="s">
@@ -4994,63 +6039,63 @@
         <v>33</v>
       </c>
       <c r="AS11" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT11" t="s">
         <v>32</v>
       </c>
       <c r="AU11" s="55">
-        <f>AK11+AE11*$E$31+AF11*$F$31+AH11*$J$31</f>
+        <f t="shared" si="4"/>
         <v>1.4839312546451142E-6</v>
       </c>
       <c r="AV11" s="56">
-        <f>(1-AK11/AU11)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW11" s="13">
         <v>9.5</v>
       </c>
       <c r="AX11" s="13">
-        <f>(($AW11/100)*(1+($AV$15+$BA11)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW11/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY11" s="13">
-        <f>$AX11/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ11" s="13">
         <v>0</v>
       </c>
       <c r="BA11" s="68">
-        <f>$AZ11/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB11" s="7"/>
       <c r="BC11" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T11*$T$32)^$T$29</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BD11" s="7" t="e">
-        <f>J11*Z11</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE11" s="8" t="e">
-        <f>BC11+((BD11-BC11)/$T$31)*F11</f>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="BF11" s="8">
-        <f>$T$27+$T$28*$T$30*(L11)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>4.944924965130653E-7</v>
       </c>
       <c r="BG11" s="7"/>
       <c r="BH11" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M11)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
+      <c r="A12" s="96"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -5077,14 +6122,14 @@
         <v>33</v>
       </c>
       <c r="J12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.894E-2</v>
       </c>
       <c r="K12" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
-      <c r="L12" s="94">
+      <c r="L12" s="91">
         <v>4.9359999623829953E-5</v>
       </c>
       <c r="M12" s="36">
@@ -5118,7 +6163,7 @@
         <v>32</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="X12" t="s">
@@ -5143,42 +6188,42 @@
         <v>33</v>
       </c>
       <c r="AE12" s="1">
-        <f>AK12*$AV$15</f>
+        <f t="shared" si="0"/>
         <v>1.2664631346800649E-3</v>
       </c>
       <c r="AF12" s="1">
-        <f>AK12*$AX12</f>
+        <f t="shared" si="1"/>
         <v>5.2209882259013124E-4</v>
       </c>
       <c r="AG12" s="24">
-        <f>AK12*$BA12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH12" s="26">
-        <f>AK12*$AY12</f>
+        <f t="shared" si="3"/>
         <v>5.2209882259013117E-3</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>2.8706497719414803E-7</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.8706497719414803E-7</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>1.4353248859707402E-9</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>1.4353248859707402E-9</v>
       </c>
       <c r="AO12" t="s">
@@ -5194,58 +6239,58 @@
         <v>33</v>
       </c>
       <c r="AS12" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="AT12" t="s">
         <v>32</v>
       </c>
       <c r="AU12" s="58">
-        <f>AK12+AE12*$E$31+AF12*$F$31+AH12*$J$31</f>
+        <f t="shared" si="4"/>
         <v>8.6145835331422058E-7</v>
       </c>
       <c r="AV12" s="57">
-        <f>(1-AK12/AU12)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AW12" s="14">
         <v>9.5</v>
       </c>
       <c r="AX12" s="13">
-        <f>(($AW12/100)*(1+($AV$15+$BA12)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AW12/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AY12" s="14">
-        <f>$AX12/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AZ12" s="14">
         <v>0</v>
       </c>
       <c r="BA12" s="68">
-        <f>$AZ12/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="BB12" s="7"/>
       <c r="BC12" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T12*$T$32)^$T$29</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BD12" s="7" t="e">
-        <f>J12*Z12</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="BE12" s="8" t="e">
-        <f>BC12+((BD12-BC12)/$T$31)*F12</f>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="BF12" s="8">
-        <f>$T$27+$T$28*$T$30*(L12)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.8706497719414803E-7</v>
       </c>
       <c r="BG12" s="7"/>
       <c r="BH12" s="7">
-        <f>$BC$20*$BB$22*$BB$24*(M12)^$BB$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5262,7 +6307,7 @@
       <c r="AF13" s="1"/>
     </row>
     <row r="14" spans="1:60" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="96" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -5363,7 +6408,7 @@
       <c r="AZ14" s="37"/>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
+      <c r="A15" s="96"/>
       <c r="B15">
         <v>1</v>
       </c>
@@ -5402,15 +6447,15 @@
         <v>1.6239747221660625</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M20" si="9">J15*$X15</f>
+        <f t="shared" ref="M15:M20" si="23">J15*$X15</f>
         <v>16.239747221660625</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N20" si="10">AA15*$J15</f>
+        <f t="shared" ref="N15:N20" si="24">AA15*$J15</f>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:O20" si="11">J15*$AB$16</f>
+        <f t="shared" ref="O15:O20" si="25">J15*$AB$16</f>
         <v>18.09675</v>
       </c>
       <c r="P15">
@@ -5436,7 +6481,7 @@
         <v>4.3</v>
       </c>
       <c r="W15" s="13">
-        <f t="shared" ref="W15:W20" si="12">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
+        <f t="shared" ref="W15:W20" si="26">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
         <v>395.90503059926971</v>
       </c>
       <c r="X15" s="13">
@@ -5450,7 +6495,7 @@
         <v>27</v>
       </c>
       <c r="AA15" s="73">
-        <f t="shared" ref="AA15:AA20" si="13">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
+        <f t="shared" ref="AA15:AA20" si="27">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="72" t="s">
@@ -5486,7 +6531,7 @@
       <c r="AZ15" s="78"/>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
+      <c r="A16" s="96"/>
       <c r="B16">
         <v>1</v>
       </c>
@@ -5517,7 +6562,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="14">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="28">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -5525,22 +6570,22 @@
         <v>0.19277131424832977</v>
       </c>
       <c r="M16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>1.9277131424832974</v>
       </c>
       <c r="N16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>7.5441176470588234</v>
       </c>
       <c r="P16">
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q16:Q20" si="15">J16*$AC16</f>
+        <f t="shared" ref="Q16:Q20" si="29">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -5560,7 +6605,7 @@
         <v>1.8</v>
       </c>
       <c r="W16" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>112.73176271832151</v>
       </c>
       <c r="X16" s="13">
@@ -5574,7 +6619,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AB16" s="42">
@@ -5582,15 +6627,15 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="13">
-        <f t="shared" ref="AC16:AC20" si="16">ROUND(X16/$AY$6*120,0)</f>
+        <f t="shared" ref="AC16:AC20" si="30">ROUND(X16/$AY$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="13">
-        <f t="shared" ref="AD16:AD20" si="17">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
+        <f t="shared" ref="AD16:AD20" si="31">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
         <v>2.1242656885690431E-3</v>
       </c>
       <c r="AE16" s="56">
-        <f t="shared" ref="AE16:AE20" si="18">(1-J16/AD16)*100</f>
+        <f t="shared" ref="AE16:AE20" si="32">(1-J16/AD16)*100</f>
         <v>19.501594871030591</v>
       </c>
       <c r="AF16" s="1"/>
@@ -5611,7 +6656,7 @@
       <c r="AZ16" s="79"/>
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+      <c r="A17" s="96"/>
       <c r="B17">
         <v>1</v>
       </c>
@@ -5642,23 +6687,23 @@
         <v>5.0624699999999995E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>2.5312349999999998E-5</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L20" si="19">J17*$W17</f>
+        <f t="shared" ref="L17:L20" si="33">J17*$W17</f>
         <v>2.3758024102824513</v>
       </c>
       <c r="M17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>23.758024102824514</v>
       </c>
       <c r="N17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>22.334426470588234</v>
       </c>
       <c r="P17">
@@ -5684,38 +6729,38 @@
         <v>4.8</v>
       </c>
       <c r="W17" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>469.29708428542818</v>
       </c>
       <c r="X17" s="13">
-        <f t="shared" ref="X17:X20" si="20">$W17/$X$23</f>
+        <f t="shared" ref="X17:X20" si="34">$W17/$X$23</f>
         <v>4692.9708428542817</v>
       </c>
       <c r="Z17" s="24"/>
       <c r="AA17" s="73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AB17" s="39">
         <v>10</v>
       </c>
       <c r="AC17" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>68</v>
       </c>
       <c r="AD17" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>8.1497066913228666E-3</v>
       </c>
       <c r="AE17" s="56">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>37.88156811348685</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A18" s="91"/>
+      <c r="A18" s="96"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -5746,30 +6791,30 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>0.36572238936056839</v>
       </c>
       <c r="M18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>3.6572238936056838</v>
       </c>
       <c r="N18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>3.0176470588235293</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>10.058823529411766</v>
       </c>
       <c r="P18">
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>5.2440000000000007E-2</v>
       </c>
       <c r="R18">
@@ -5789,11 +6834,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W18" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X18" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="34"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA18" s="73">
@@ -5804,22 +6849,22 @@
         <v>104</v>
       </c>
       <c r="AC18" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="AD18" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>2.9444020852838065E-3</v>
       </c>
       <c r="AE18" s="56">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>22.564923744773314</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A19" s="91"/>
+      <c r="A19" s="96"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -5850,30 +6895,30 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>6.4161822694836562E-3</v>
       </c>
       <c r="M19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>6.4161822694836557E-2</v>
       </c>
       <c r="N19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="P19">
         <v>4.7099999999999998E-6</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="R19">
@@ -5893,28 +6938,28 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W19" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X19" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="34"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA19" s="73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="AD19" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>5.1656176934803615E-5</v>
       </c>
       <c r="AE19" s="56">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>22.564923744773303</v>
       </c>
       <c r="BA19" s="63" t="s">
@@ -5928,7 +6973,7 @@
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A20" s="91"/>
+      <c r="A20" s="96"/>
       <c r="B20">
         <v>1</v>
       </c>
@@ -5958,30 +7003,30 @@
         <v>4.0322099999999996E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>2.0161049999999999E-5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>2.0843008232103681</v>
       </c>
       <c r="M20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>20.843008232103678</v>
       </c>
       <c r="N20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>17.789161764705881</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>0.30241574999999998</v>
       </c>
       <c r="R20">
@@ -6000,27 +7045,27 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="W20" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>516.91276575633913</v>
       </c>
       <c r="X20" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="34"/>
         <v>5169.127657563391</v>
       </c>
       <c r="AA20" s="74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AC20" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>75</v>
       </c>
       <c r="AD20" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>6.689085819105817E-3</v>
       </c>
       <c r="AE20" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>39.719565437732463</v>
       </c>
       <c r="BA20" s="63"/>
@@ -6148,7 +7193,7 @@
       </c>
     </row>
     <row r="25" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A25" s="91" t="s">
+      <c r="A25" s="96" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -6209,7 +7254,7 @@
       </c>
     </row>
     <row r="26" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A26" s="91"/>
+      <c r="A26" s="96"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -6263,7 +7308,7 @@
       <c r="BA26" s="7"/>
     </row>
     <row r="27" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
+      <c r="A27" s="96"/>
       <c r="B27">
         <v>1</v>
       </c>
@@ -6318,7 +7363,7 @@
       <c r="Q27" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="R27" s="92" t="s">
+      <c r="R27" s="97" t="s">
         <v>46</v>
       </c>
       <c r="S27" s="7" t="s">
@@ -6377,7 +7422,7 @@
       <c r="Q28" s="14">
         <v>1.2</v>
       </c>
-      <c r="R28" s="92"/>
+      <c r="R28" s="97"/>
       <c r="S28" s="7" t="s">
         <v>48</v>
       </c>
@@ -6404,7 +7449,7 @@
     </row>
     <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
-      <c r="R29" s="92"/>
+      <c r="R29" s="97"/>
       <c r="S29" s="7" t="s">
         <v>49</v>
       </c>
@@ -6447,7 +7492,7 @@
         <f>K27+SUM(J15:J20)+SUM(AK5:AK12)</f>
         <v>5.3967520737202901E-2</v>
       </c>
-      <c r="R30" s="92"/>
+      <c r="R30" s="97"/>
       <c r="S30" s="7" t="s">
         <v>50</v>
       </c>
@@ -6496,7 +7541,7 @@
         <f>( 0.000001*14) / 0.151</f>
         <v>9.2715231788079476E-5</v>
       </c>
-      <c r="R31" s="92"/>
+      <c r="R31" s="97"/>
       <c r="S31" s="7" t="s">
         <v>51</v>
       </c>
@@ -6548,7 +7593,7 @@
         <f>E26*E31+F26*F31</f>
         <v>0</v>
       </c>
-      <c r="R32" s="92"/>
+      <c r="R32" s="97"/>
       <c r="S32" s="9" t="s">
         <v>52</v>
       </c>
@@ -6587,7 +7632,7 @@
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="93" t="s">
+      <c r="A35" s="98" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -6636,7 +7681,7 @@
       <c r="Q35" s="25"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="93"/>
+      <c r="A36" s="98"/>
       <c r="B36">
         <v>1</v>
       </c>
@@ -6931,4 +7976,343 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="93" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="94" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="92" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>-2.0999999999999999E-3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8">
+        <v>-0.1527</v>
+      </c>
+      <c r="C8">
+        <v>1.763E-2</v>
+      </c>
+      <c r="D8">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9">
+        <v>0.49619999999999997</v>
+      </c>
+      <c r="C9">
+        <v>0.25</v>
+      </c>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f>$B$6*$A13^3 + $B$7*$A13^2 + $B$8*$A13 + $B$9</f>
+        <v>0.37839999999999996</v>
+      </c>
+      <c r="C13">
+        <f>$C$6*$A13^3 + $C$7*$A13^2 + $C$8*$A13 + $C$9</f>
+        <v>0.26762999999999998</v>
+      </c>
+      <c r="D13">
+        <f>$D$6*$A13^3 + $D$7*$A13^2 + $D$8*$A13 + $D$9</f>
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B26" si="0">$B$6*$A14^3 + $B$7*$A14^2 + $B$8*$A14 + $B$9</f>
+        <v>0.32199999999999995</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C26" si="1">$C$6*$A14^3 + $C$7*$A14^2 + $C$8*$A14 + $C$9</f>
+        <v>0.28526000000000001</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D26" si="2">$D$6*$A14^3 + $D$7*$A14^2 + $D$8*$A14 + $D$9</f>
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.31439999999999996</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.30288999999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.33599999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.34299999999999997</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.32052000000000003</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.39519999999999977</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.33815000000000001</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.45839999999999981</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.35577999999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.37341000000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.5673999999999999</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.39104</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.58799999999999986</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.40866999999999998</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.56919999999999948</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.42630000000000001</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.49839999999999973</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.44392999999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>0.432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.36299999999999977</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.46155999999999997</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.15040000000000031</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.47919</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0.45599999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>-0.15199999999999969</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.49681999999999998</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>0.46799999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>